<commit_message>
all: update report BELINVENTORY_BARCODE_2022 and fix bug with import
</commit_message>
<xml_diff>
--- a/templates/BELINVENTORY_BARCODE_2022.xlsx
+++ b/templates/BELINVENTORY_BARCODE_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexb\source\repos\parus-electronic-inventory-app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBFD5EA-538D-423A-A59E-D897CB4EB241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825F4D5-7D62-4173-BB5E-7FC56D0BB99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="1785" windowWidth="21135" windowHeight="12720" xr2:uid="{E480F2B1-D09D-481B-863B-42622AF3855B}"/>
   </bookViews>
@@ -546,7 +546,9 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -568,7 +570,7 @@
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:3" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="7" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>

</xml_diff>